<commit_message>
RDM-2804-Added And conditions functional tests
</commit_message>
<xml_diff>
--- a/test/resources/definitionsFiles/fe-automation-definition-v06_collection_view_2804.xlsx
+++ b/test/resources/definitionsFiles/fe-automation-definition-v06_collection_view_2804.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ganganna/moj/code/ccd-case-management-web/test/resources/definitionsFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F9DDB6-BB37-9646-A715-94FAA403CF0C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B459D626-3BDC-1947-85CC-29DDDEB38C48}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="520" windowWidth="28600" windowHeight="17380" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2167" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2239" uniqueCount="516">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1642,6 +1642,33 @@
   </si>
   <si>
     <t>TextField6!="orValue1" OR TextField6!="orValue2"</t>
+  </si>
+  <si>
+    <t>createCaseAnd</t>
+  </si>
+  <si>
+    <t>Create a case AND</t>
+  </si>
+  <si>
+    <t>TextField8</t>
+  </si>
+  <si>
+    <t>TextField9</t>
+  </si>
+  <si>
+    <t>TextField10</t>
+  </si>
+  <si>
+    <t>Text Field 8</t>
+  </si>
+  <si>
+    <t>Text Field 9</t>
+  </si>
+  <si>
+    <t>Text Field 10</t>
+  </si>
+  <si>
+    <t>TextField8="orValue1" AND TextField9="orValue2"</t>
   </si>
 </sst>
 </file>
@@ -3602,10 +3629,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AD51"/>
+  <dimension ref="A1:AD55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C18" workbookViewId="0">
-      <selection activeCell="I57" sqref="I57"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B23" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3613,11 +3640,11 @@
     <col min="1" max="1" width="22.6640625" style="22" customWidth="1"/>
     <col min="2" max="2" width="15.5" style="22" customWidth="1"/>
     <col min="3" max="3" width="24.6640625" style="22" customWidth="1"/>
-    <col min="4" max="4" width="21" style="22" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" style="22" customWidth="1"/>
+    <col min="4" max="4" width="27.83203125" style="22" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" style="22" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="22" customWidth="1"/>
     <col min="7" max="7" width="14.83203125" style="22" customWidth="1"/>
-    <col min="8" max="8" width="19.6640625" style="22" customWidth="1"/>
+    <col min="8" max="8" width="28.6640625" style="22" customWidth="1"/>
     <col min="9" max="9" width="22" style="22" customWidth="1"/>
     <col min="10" max="10" width="11.5" style="22" customWidth="1"/>
     <col min="11" max="11" width="12.6640625" style="22" customWidth="1"/>
@@ -6006,7 +6033,7 @@
         <v>336</v>
       </c>
       <c r="F47" s="23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G47" s="8" t="s">
         <v>218</v>
@@ -6163,7 +6190,7 @@
         <v>339</v>
       </c>
       <c r="F50" s="23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G50" s="8" t="s">
         <v>218</v>
@@ -6253,6 +6280,214 @@
       <c r="AA51" s="7"/>
       <c r="AB51" s="7"/>
       <c r="AC51" s="7"/>
+    </row>
+    <row r="52" spans="1:29" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B52" s="10"/>
+      <c r="C52" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>507</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>509</v>
+      </c>
+      <c r="F52" s="23">
+        <v>1</v>
+      </c>
+      <c r="G52" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="H52" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="I52" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="J52" s="6">
+        <v>1</v>
+      </c>
+      <c r="K52" s="7"/>
+      <c r="L52" s="7"/>
+      <c r="M52" s="7"/>
+      <c r="N52" s="142"/>
+      <c r="O52" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="P52" s="7"/>
+      <c r="Q52" s="7"/>
+      <c r="R52" s="7"/>
+      <c r="S52" s="7"/>
+      <c r="T52" s="7"/>
+      <c r="U52" s="7"/>
+      <c r="V52" s="7"/>
+      <c r="W52" s="7"/>
+      <c r="X52" s="7"/>
+      <c r="Y52" s="7"/>
+      <c r="Z52" s="7"/>
+      <c r="AA52" s="7"/>
+      <c r="AB52" s="7"/>
+      <c r="AC52" s="7"/>
+    </row>
+    <row r="53" spans="1:29" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A53" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B53" s="10"/>
+      <c r="C53" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>507</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>510</v>
+      </c>
+      <c r="F53" s="23">
+        <v>1</v>
+      </c>
+      <c r="G53" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="H53" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="I53" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="J53" s="6">
+        <v>1</v>
+      </c>
+      <c r="K53" s="7"/>
+      <c r="L53" s="7"/>
+      <c r="M53" s="7"/>
+      <c r="N53" s="142"/>
+      <c r="O53" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="P53" s="7"/>
+      <c r="Q53" s="7"/>
+      <c r="R53" s="7"/>
+      <c r="S53" s="7"/>
+      <c r="T53" s="7"/>
+      <c r="U53" s="7"/>
+      <c r="V53" s="7"/>
+      <c r="W53" s="7"/>
+      <c r="X53" s="7"/>
+      <c r="Y53" s="7"/>
+      <c r="Z53" s="7"/>
+      <c r="AA53" s="7"/>
+      <c r="AB53" s="7"/>
+      <c r="AC53" s="7"/>
+    </row>
+    <row r="54" spans="1:29" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A54" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B54" s="10"/>
+      <c r="C54" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>507</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>511</v>
+      </c>
+      <c r="F54" s="23">
+        <v>2</v>
+      </c>
+      <c r="G54" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="H54" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="I54" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="J54" s="6">
+        <v>2</v>
+      </c>
+      <c r="K54" s="7"/>
+      <c r="L54" s="7"/>
+      <c r="M54" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="N54" s="142"/>
+      <c r="O54" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="P54" s="7"/>
+      <c r="Q54" s="7"/>
+      <c r="R54" s="7"/>
+      <c r="S54" s="7"/>
+      <c r="T54" s="7"/>
+      <c r="U54" s="7"/>
+      <c r="V54" s="7"/>
+      <c r="W54" s="7"/>
+      <c r="X54" s="7"/>
+      <c r="Y54" s="7"/>
+      <c r="Z54" s="7"/>
+      <c r="AA54" s="7"/>
+      <c r="AB54" s="7"/>
+      <c r="AC54" s="7"/>
+    </row>
+    <row r="55" spans="1:29" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A55" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B55" s="10"/>
+      <c r="C55" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>507</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>496</v>
+      </c>
+      <c r="F55" s="23">
+        <v>2</v>
+      </c>
+      <c r="G55" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="H55" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="I55" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="J55" s="6">
+        <v>1</v>
+      </c>
+      <c r="K55" s="7"/>
+      <c r="L55" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="M55" s="7"/>
+      <c r="N55" s="142"/>
+      <c r="O55" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="P55" s="7"/>
+      <c r="Q55" s="7"/>
+      <c r="R55" s="7"/>
+      <c r="S55" s="7"/>
+      <c r="T55" s="7"/>
+      <c r="U55" s="7"/>
+      <c r="V55" s="7"/>
+      <c r="W55" s="7"/>
+      <c r="X55" s="7"/>
+      <c r="Y55" s="7"/>
+      <c r="Z55" s="7"/>
+      <c r="AA55" s="7"/>
+      <c r="AB55" s="7"/>
+      <c r="AC55" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
@@ -7900,10 +8135,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:IV55"/>
+  <dimension ref="A1:IV59"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+    <sheetView showGridLines="0" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10130,6 +10365,98 @@
       <c r="J55" s="7"/>
       <c r="K55" s="7"/>
     </row>
+    <row r="56" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A56" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B56" s="10"/>
+      <c r="C56" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="D56" s="57" t="s">
+        <v>339</v>
+      </c>
+      <c r="E56" t="s">
+        <v>271</v>
+      </c>
+      <c r="F56" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="G56" s="8"/>
+      <c r="H56" s="7"/>
+      <c r="I56" s="7"/>
+      <c r="J56" s="7"/>
+      <c r="K56" s="7"/>
+    </row>
+    <row r="57" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A57" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B57" s="10"/>
+      <c r="C57" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="D57" s="57" t="s">
+        <v>509</v>
+      </c>
+      <c r="E57" t="s">
+        <v>271</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="G57" s="8"/>
+      <c r="H57" s="7"/>
+      <c r="I57" s="7"/>
+      <c r="J57" s="7"/>
+      <c r="K57" s="7"/>
+    </row>
+    <row r="58" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A58" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B58" s="10"/>
+      <c r="C58" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="D58" s="57" t="s">
+        <v>510</v>
+      </c>
+      <c r="E58" t="s">
+        <v>271</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="G58" s="8"/>
+      <c r="H58" s="7"/>
+      <c r="I58" s="7"/>
+      <c r="J58" s="7"/>
+      <c r="K58" s="7"/>
+    </row>
+    <row r="59" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A59" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B59" s="10"/>
+      <c r="C59" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="D59" s="57" t="s">
+        <v>511</v>
+      </c>
+      <c r="E59" t="s">
+        <v>271</v>
+      </c>
+      <c r="F59" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="G59" s="8"/>
+      <c r="H59" s="7"/>
+      <c r="I59" s="7"/>
+      <c r="J59" s="7"/>
+      <c r="K59" s="7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -10257,10 +10584,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10758,6 +11085,29 @@
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
+    </row>
+    <row r="22" spans="1:11" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B22" s="7"/>
+      <c r="C22" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>507</v>
+      </c>
+      <c r="E22" s="54" t="s">
+        <v>271</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
@@ -11447,10 +11797,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:IV57"/>
+  <dimension ref="A1:IV60"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView showGridLines="0" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -23313,6 +23663,816 @@
       <c r="IU57" s="92"/>
       <c r="IV57" s="92"/>
     </row>
+    <row r="58" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A58" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B58" s="10"/>
+      <c r="C58" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>509</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>512</v>
+      </c>
+      <c r="F58" s="7"/>
+      <c r="G58" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H58" s="7"/>
+      <c r="I58" s="7"/>
+      <c r="J58" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K58" s="7"/>
+      <c r="L58" s="7"/>
+      <c r="M58" s="7"/>
+      <c r="N58" s="7"/>
+      <c r="O58" s="7"/>
+      <c r="P58" s="7"/>
+      <c r="Q58" s="7"/>
+      <c r="R58" s="42"/>
+      <c r="S58" s="42"/>
+      <c r="T58" s="42"/>
+      <c r="U58" s="42"/>
+      <c r="V58" s="42"/>
+      <c r="W58" s="42"/>
+      <c r="X58" s="42"/>
+      <c r="Y58" s="42"/>
+      <c r="Z58" s="42"/>
+      <c r="AA58" s="42"/>
+      <c r="AB58" s="42"/>
+      <c r="AC58" s="42"/>
+      <c r="AD58" s="42"/>
+      <c r="AE58" s="42"/>
+      <c r="AF58" s="42"/>
+      <c r="AG58" s="42"/>
+      <c r="AH58" s="42"/>
+      <c r="AI58" s="42"/>
+      <c r="AJ58" s="42"/>
+      <c r="AK58" s="42"/>
+      <c r="AL58" s="42"/>
+      <c r="AM58" s="42"/>
+      <c r="AN58" s="42"/>
+      <c r="AO58" s="42"/>
+      <c r="AP58" s="42"/>
+      <c r="AQ58" s="42"/>
+      <c r="AR58" s="42"/>
+      <c r="AS58" s="42"/>
+      <c r="AT58" s="42"/>
+      <c r="AU58" s="42"/>
+      <c r="AV58" s="42"/>
+      <c r="AW58" s="42"/>
+      <c r="AX58" s="42"/>
+      <c r="AY58" s="42"/>
+      <c r="AZ58" s="42"/>
+      <c r="BA58" s="42"/>
+      <c r="BB58" s="42"/>
+      <c r="BC58" s="42"/>
+      <c r="BD58" s="42"/>
+      <c r="BE58" s="42"/>
+      <c r="BF58" s="42"/>
+      <c r="BG58" s="42"/>
+      <c r="BH58" s="42"/>
+      <c r="BI58" s="42"/>
+      <c r="BJ58" s="42"/>
+      <c r="BK58" s="42"/>
+      <c r="BL58" s="42"/>
+      <c r="BM58" s="42"/>
+      <c r="BN58" s="42"/>
+      <c r="BO58" s="42"/>
+      <c r="BP58" s="42"/>
+      <c r="BQ58" s="42"/>
+      <c r="BR58" s="42"/>
+      <c r="BS58" s="42"/>
+      <c r="BT58" s="42"/>
+      <c r="BU58" s="42"/>
+      <c r="BV58" s="42"/>
+      <c r="BW58" s="42"/>
+      <c r="BX58" s="42"/>
+      <c r="BY58" s="42"/>
+      <c r="BZ58" s="42"/>
+      <c r="CA58" s="42"/>
+      <c r="CB58" s="42"/>
+      <c r="CC58" s="42"/>
+      <c r="CD58" s="42"/>
+      <c r="CE58" s="42"/>
+      <c r="CF58" s="42"/>
+      <c r="CG58" s="42"/>
+      <c r="CH58" s="42"/>
+      <c r="CI58" s="42"/>
+      <c r="CJ58" s="42"/>
+      <c r="CK58" s="42"/>
+      <c r="CL58" s="42"/>
+      <c r="CM58" s="42"/>
+      <c r="CN58" s="42"/>
+      <c r="CO58" s="42"/>
+      <c r="CP58" s="42"/>
+      <c r="CQ58" s="42"/>
+      <c r="CR58" s="42"/>
+      <c r="CS58" s="42"/>
+      <c r="CT58" s="42"/>
+      <c r="CU58" s="42"/>
+      <c r="CV58" s="42"/>
+      <c r="CW58" s="42"/>
+      <c r="CX58" s="42"/>
+      <c r="CY58" s="42"/>
+      <c r="CZ58" s="42"/>
+      <c r="DA58" s="42"/>
+      <c r="DB58" s="42"/>
+      <c r="DC58" s="42"/>
+      <c r="DD58" s="42"/>
+      <c r="DE58" s="42"/>
+      <c r="DF58" s="42"/>
+      <c r="DG58" s="42"/>
+      <c r="DH58" s="42"/>
+      <c r="DI58" s="42"/>
+      <c r="DJ58" s="42"/>
+      <c r="DK58" s="42"/>
+      <c r="DL58" s="42"/>
+      <c r="DM58" s="42"/>
+      <c r="DN58" s="42"/>
+      <c r="DO58" s="42"/>
+      <c r="DP58" s="42"/>
+      <c r="DQ58" s="42"/>
+      <c r="DR58" s="42"/>
+      <c r="DS58" s="42"/>
+      <c r="DT58" s="42"/>
+      <c r="DU58" s="42"/>
+      <c r="DV58" s="42"/>
+      <c r="DW58" s="42"/>
+      <c r="DX58" s="42"/>
+      <c r="DY58" s="42"/>
+      <c r="DZ58" s="42"/>
+      <c r="EA58" s="42"/>
+      <c r="EB58" s="42"/>
+      <c r="EC58" s="42"/>
+      <c r="ED58" s="42"/>
+      <c r="EE58" s="42"/>
+      <c r="EF58" s="42"/>
+      <c r="EG58" s="42"/>
+      <c r="EH58" s="42"/>
+      <c r="EI58" s="42"/>
+      <c r="EJ58" s="42"/>
+      <c r="EK58" s="42"/>
+      <c r="EL58" s="42"/>
+      <c r="EM58" s="42"/>
+      <c r="EN58" s="42"/>
+      <c r="EO58" s="42"/>
+      <c r="EP58" s="42"/>
+      <c r="EQ58" s="42"/>
+      <c r="ER58" s="42"/>
+      <c r="ES58" s="42"/>
+      <c r="ET58" s="42"/>
+      <c r="EU58" s="42"/>
+      <c r="EV58" s="42"/>
+      <c r="EW58" s="42"/>
+      <c r="EX58" s="42"/>
+      <c r="EY58" s="42"/>
+      <c r="EZ58" s="42"/>
+      <c r="FA58" s="42"/>
+      <c r="FB58" s="42"/>
+      <c r="FC58" s="42"/>
+      <c r="FD58" s="42"/>
+      <c r="FE58" s="42"/>
+      <c r="FF58" s="42"/>
+      <c r="FG58" s="42"/>
+      <c r="FH58" s="42"/>
+      <c r="FI58" s="42"/>
+      <c r="FJ58" s="42"/>
+      <c r="FK58" s="42"/>
+      <c r="FL58" s="42"/>
+      <c r="FM58" s="42"/>
+      <c r="FN58" s="42"/>
+      <c r="FO58" s="42"/>
+      <c r="FP58" s="42"/>
+      <c r="FQ58" s="42"/>
+      <c r="FR58" s="42"/>
+      <c r="FS58" s="42"/>
+      <c r="FT58" s="42"/>
+      <c r="FU58" s="42"/>
+      <c r="FV58" s="42"/>
+      <c r="FW58" s="42"/>
+      <c r="FX58" s="42"/>
+      <c r="FY58" s="42"/>
+      <c r="FZ58" s="42"/>
+      <c r="GA58" s="42"/>
+      <c r="GB58" s="42"/>
+      <c r="GC58" s="42"/>
+      <c r="GD58" s="42"/>
+      <c r="GE58" s="42"/>
+      <c r="GF58" s="42"/>
+      <c r="GG58" s="42"/>
+      <c r="GH58" s="42"/>
+      <c r="GI58" s="42"/>
+      <c r="GJ58" s="42"/>
+      <c r="GK58" s="42"/>
+      <c r="GL58" s="42"/>
+      <c r="GM58" s="42"/>
+      <c r="GN58" s="42"/>
+      <c r="GO58" s="42"/>
+      <c r="GP58" s="42"/>
+      <c r="GQ58" s="42"/>
+      <c r="GR58" s="42"/>
+      <c r="GS58" s="42"/>
+      <c r="GT58" s="42"/>
+      <c r="GU58" s="42"/>
+      <c r="GV58" s="42"/>
+      <c r="GW58" s="42"/>
+      <c r="GX58" s="42"/>
+      <c r="GY58" s="42"/>
+      <c r="GZ58" s="42"/>
+      <c r="HA58" s="42"/>
+      <c r="HB58" s="42"/>
+      <c r="HC58" s="42"/>
+      <c r="HD58" s="42"/>
+      <c r="HE58" s="42"/>
+      <c r="HF58" s="42"/>
+      <c r="HG58" s="42"/>
+      <c r="HH58" s="42"/>
+      <c r="HI58" s="42"/>
+      <c r="HJ58" s="42"/>
+      <c r="HK58" s="42"/>
+      <c r="HL58" s="42"/>
+      <c r="HM58" s="42"/>
+      <c r="HN58" s="42"/>
+      <c r="HO58" s="42"/>
+      <c r="HP58" s="42"/>
+      <c r="HQ58" s="42"/>
+      <c r="HR58" s="42"/>
+      <c r="HS58" s="42"/>
+      <c r="HT58" s="42"/>
+      <c r="HU58" s="42"/>
+      <c r="HV58" s="42"/>
+      <c r="HW58" s="42"/>
+      <c r="HX58" s="42"/>
+      <c r="HY58" s="42"/>
+      <c r="HZ58" s="42"/>
+      <c r="IA58" s="42"/>
+      <c r="IB58" s="42"/>
+      <c r="IC58" s="42"/>
+      <c r="ID58" s="42"/>
+      <c r="IE58" s="42"/>
+      <c r="IF58" s="42"/>
+      <c r="IG58" s="42"/>
+      <c r="IH58" s="42"/>
+      <c r="II58" s="42"/>
+      <c r="IJ58" s="42"/>
+      <c r="IK58" s="42"/>
+      <c r="IL58" s="42"/>
+      <c r="IM58" s="42"/>
+      <c r="IN58" s="42"/>
+      <c r="IO58" s="42"/>
+      <c r="IP58" s="42"/>
+      <c r="IQ58" s="42"/>
+      <c r="IR58" s="42"/>
+      <c r="IS58" s="42"/>
+      <c r="IT58" s="42"/>
+      <c r="IU58" s="42"/>
+      <c r="IV58" s="42"/>
+    </row>
+    <row r="59" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A59" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B59" s="10"/>
+      <c r="C59" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>510</v>
+      </c>
+      <c r="E59" s="8" t="s">
+        <v>513</v>
+      </c>
+      <c r="F59" s="7"/>
+      <c r="G59" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H59" s="7"/>
+      <c r="I59" s="7"/>
+      <c r="J59" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K59" s="7"/>
+      <c r="L59" s="7"/>
+      <c r="M59" s="7"/>
+      <c r="N59" s="7"/>
+      <c r="O59" s="7"/>
+      <c r="P59" s="7"/>
+      <c r="Q59" s="7"/>
+      <c r="R59" s="42"/>
+      <c r="S59" s="42"/>
+      <c r="T59" s="42"/>
+      <c r="U59" s="42"/>
+      <c r="V59" s="42"/>
+      <c r="W59" s="42"/>
+      <c r="X59" s="42"/>
+      <c r="Y59" s="42"/>
+      <c r="Z59" s="42"/>
+      <c r="AA59" s="42"/>
+      <c r="AB59" s="42"/>
+      <c r="AC59" s="42"/>
+      <c r="AD59" s="42"/>
+      <c r="AE59" s="42"/>
+      <c r="AF59" s="42"/>
+      <c r="AG59" s="42"/>
+      <c r="AH59" s="42"/>
+      <c r="AI59" s="42"/>
+      <c r="AJ59" s="42"/>
+      <c r="AK59" s="42"/>
+      <c r="AL59" s="42"/>
+      <c r="AM59" s="42"/>
+      <c r="AN59" s="42"/>
+      <c r="AO59" s="42"/>
+      <c r="AP59" s="42"/>
+      <c r="AQ59" s="42"/>
+      <c r="AR59" s="42"/>
+      <c r="AS59" s="42"/>
+      <c r="AT59" s="42"/>
+      <c r="AU59" s="42"/>
+      <c r="AV59" s="42"/>
+      <c r="AW59" s="42"/>
+      <c r="AX59" s="42"/>
+      <c r="AY59" s="42"/>
+      <c r="AZ59" s="42"/>
+      <c r="BA59" s="42"/>
+      <c r="BB59" s="42"/>
+      <c r="BC59" s="42"/>
+      <c r="BD59" s="42"/>
+      <c r="BE59" s="42"/>
+      <c r="BF59" s="42"/>
+      <c r="BG59" s="42"/>
+      <c r="BH59" s="42"/>
+      <c r="BI59" s="42"/>
+      <c r="BJ59" s="42"/>
+      <c r="BK59" s="42"/>
+      <c r="BL59" s="42"/>
+      <c r="BM59" s="42"/>
+      <c r="BN59" s="42"/>
+      <c r="BO59" s="42"/>
+      <c r="BP59" s="42"/>
+      <c r="BQ59" s="42"/>
+      <c r="BR59" s="42"/>
+      <c r="BS59" s="42"/>
+      <c r="BT59" s="42"/>
+      <c r="BU59" s="42"/>
+      <c r="BV59" s="42"/>
+      <c r="BW59" s="42"/>
+      <c r="BX59" s="42"/>
+      <c r="BY59" s="42"/>
+      <c r="BZ59" s="42"/>
+      <c r="CA59" s="42"/>
+      <c r="CB59" s="42"/>
+      <c r="CC59" s="42"/>
+      <c r="CD59" s="42"/>
+      <c r="CE59" s="42"/>
+      <c r="CF59" s="42"/>
+      <c r="CG59" s="42"/>
+      <c r="CH59" s="42"/>
+      <c r="CI59" s="42"/>
+      <c r="CJ59" s="42"/>
+      <c r="CK59" s="42"/>
+      <c r="CL59" s="42"/>
+      <c r="CM59" s="42"/>
+      <c r="CN59" s="42"/>
+      <c r="CO59" s="42"/>
+      <c r="CP59" s="42"/>
+      <c r="CQ59" s="42"/>
+      <c r="CR59" s="42"/>
+      <c r="CS59" s="42"/>
+      <c r="CT59" s="42"/>
+      <c r="CU59" s="42"/>
+      <c r="CV59" s="42"/>
+      <c r="CW59" s="42"/>
+      <c r="CX59" s="42"/>
+      <c r="CY59" s="42"/>
+      <c r="CZ59" s="42"/>
+      <c r="DA59" s="42"/>
+      <c r="DB59" s="42"/>
+      <c r="DC59" s="42"/>
+      <c r="DD59" s="42"/>
+      <c r="DE59" s="42"/>
+      <c r="DF59" s="42"/>
+      <c r="DG59" s="42"/>
+      <c r="DH59" s="42"/>
+      <c r="DI59" s="42"/>
+      <c r="DJ59" s="42"/>
+      <c r="DK59" s="42"/>
+      <c r="DL59" s="42"/>
+      <c r="DM59" s="42"/>
+      <c r="DN59" s="42"/>
+      <c r="DO59" s="42"/>
+      <c r="DP59" s="42"/>
+      <c r="DQ59" s="42"/>
+      <c r="DR59" s="42"/>
+      <c r="DS59" s="42"/>
+      <c r="DT59" s="42"/>
+      <c r="DU59" s="42"/>
+      <c r="DV59" s="42"/>
+      <c r="DW59" s="42"/>
+      <c r="DX59" s="42"/>
+      <c r="DY59" s="42"/>
+      <c r="DZ59" s="42"/>
+      <c r="EA59" s="42"/>
+      <c r="EB59" s="42"/>
+      <c r="EC59" s="42"/>
+      <c r="ED59" s="42"/>
+      <c r="EE59" s="42"/>
+      <c r="EF59" s="42"/>
+      <c r="EG59" s="42"/>
+      <c r="EH59" s="42"/>
+      <c r="EI59" s="42"/>
+      <c r="EJ59" s="42"/>
+      <c r="EK59" s="42"/>
+      <c r="EL59" s="42"/>
+      <c r="EM59" s="42"/>
+      <c r="EN59" s="42"/>
+      <c r="EO59" s="42"/>
+      <c r="EP59" s="42"/>
+      <c r="EQ59" s="42"/>
+      <c r="ER59" s="42"/>
+      <c r="ES59" s="42"/>
+      <c r="ET59" s="42"/>
+      <c r="EU59" s="42"/>
+      <c r="EV59" s="42"/>
+      <c r="EW59" s="42"/>
+      <c r="EX59" s="42"/>
+      <c r="EY59" s="42"/>
+      <c r="EZ59" s="42"/>
+      <c r="FA59" s="42"/>
+      <c r="FB59" s="42"/>
+      <c r="FC59" s="42"/>
+      <c r="FD59" s="42"/>
+      <c r="FE59" s="42"/>
+      <c r="FF59" s="42"/>
+      <c r="FG59" s="42"/>
+      <c r="FH59" s="42"/>
+      <c r="FI59" s="42"/>
+      <c r="FJ59" s="42"/>
+      <c r="FK59" s="42"/>
+      <c r="FL59" s="42"/>
+      <c r="FM59" s="42"/>
+      <c r="FN59" s="42"/>
+      <c r="FO59" s="42"/>
+      <c r="FP59" s="42"/>
+      <c r="FQ59" s="42"/>
+      <c r="FR59" s="42"/>
+      <c r="FS59" s="42"/>
+      <c r="FT59" s="42"/>
+      <c r="FU59" s="42"/>
+      <c r="FV59" s="42"/>
+      <c r="FW59" s="42"/>
+      <c r="FX59" s="42"/>
+      <c r="FY59" s="42"/>
+      <c r="FZ59" s="42"/>
+      <c r="GA59" s="42"/>
+      <c r="GB59" s="42"/>
+      <c r="GC59" s="42"/>
+      <c r="GD59" s="42"/>
+      <c r="GE59" s="42"/>
+      <c r="GF59" s="42"/>
+      <c r="GG59" s="42"/>
+      <c r="GH59" s="42"/>
+      <c r="GI59" s="42"/>
+      <c r="GJ59" s="42"/>
+      <c r="GK59" s="42"/>
+      <c r="GL59" s="42"/>
+      <c r="GM59" s="42"/>
+      <c r="GN59" s="42"/>
+      <c r="GO59" s="42"/>
+      <c r="GP59" s="42"/>
+      <c r="GQ59" s="42"/>
+      <c r="GR59" s="42"/>
+      <c r="GS59" s="42"/>
+      <c r="GT59" s="42"/>
+      <c r="GU59" s="42"/>
+      <c r="GV59" s="42"/>
+      <c r="GW59" s="42"/>
+      <c r="GX59" s="42"/>
+      <c r="GY59" s="42"/>
+      <c r="GZ59" s="42"/>
+      <c r="HA59" s="42"/>
+      <c r="HB59" s="42"/>
+      <c r="HC59" s="42"/>
+      <c r="HD59" s="42"/>
+      <c r="HE59" s="42"/>
+      <c r="HF59" s="42"/>
+      <c r="HG59" s="42"/>
+      <c r="HH59" s="42"/>
+      <c r="HI59" s="42"/>
+      <c r="HJ59" s="42"/>
+      <c r="HK59" s="42"/>
+      <c r="HL59" s="42"/>
+      <c r="HM59" s="42"/>
+      <c r="HN59" s="42"/>
+      <c r="HO59" s="42"/>
+      <c r="HP59" s="42"/>
+      <c r="HQ59" s="42"/>
+      <c r="HR59" s="42"/>
+      <c r="HS59" s="42"/>
+      <c r="HT59" s="42"/>
+      <c r="HU59" s="42"/>
+      <c r="HV59" s="42"/>
+      <c r="HW59" s="42"/>
+      <c r="HX59" s="42"/>
+      <c r="HY59" s="42"/>
+      <c r="HZ59" s="42"/>
+      <c r="IA59" s="42"/>
+      <c r="IB59" s="42"/>
+      <c r="IC59" s="42"/>
+      <c r="ID59" s="42"/>
+      <c r="IE59" s="42"/>
+      <c r="IF59" s="42"/>
+      <c r="IG59" s="42"/>
+      <c r="IH59" s="42"/>
+      <c r="II59" s="42"/>
+      <c r="IJ59" s="42"/>
+      <c r="IK59" s="42"/>
+      <c r="IL59" s="42"/>
+      <c r="IM59" s="42"/>
+      <c r="IN59" s="42"/>
+      <c r="IO59" s="42"/>
+      <c r="IP59" s="42"/>
+      <c r="IQ59" s="42"/>
+      <c r="IR59" s="42"/>
+      <c r="IS59" s="42"/>
+      <c r="IT59" s="42"/>
+      <c r="IU59" s="42"/>
+      <c r="IV59" s="42"/>
+    </row>
+    <row r="60" spans="1:256" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A60" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B60" s="10"/>
+      <c r="C60" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>511</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>514</v>
+      </c>
+      <c r="F60" s="7"/>
+      <c r="G60" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H60" s="7"/>
+      <c r="I60" s="7"/>
+      <c r="J60" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K60" s="7"/>
+      <c r="L60" s="7"/>
+      <c r="M60" s="7"/>
+      <c r="N60" s="7"/>
+      <c r="O60" s="7"/>
+      <c r="P60" s="7"/>
+      <c r="Q60" s="7"/>
+      <c r="R60" s="42"/>
+      <c r="S60" s="42"/>
+      <c r="T60" s="42"/>
+      <c r="U60" s="42"/>
+      <c r="V60" s="42"/>
+      <c r="W60" s="42"/>
+      <c r="X60" s="42"/>
+      <c r="Y60" s="42"/>
+      <c r="Z60" s="42"/>
+      <c r="AA60" s="42"/>
+      <c r="AB60" s="42"/>
+      <c r="AC60" s="42"/>
+      <c r="AD60" s="42"/>
+      <c r="AE60" s="42"/>
+      <c r="AF60" s="42"/>
+      <c r="AG60" s="42"/>
+      <c r="AH60" s="42"/>
+      <c r="AI60" s="42"/>
+      <c r="AJ60" s="42"/>
+      <c r="AK60" s="42"/>
+      <c r="AL60" s="42"/>
+      <c r="AM60" s="42"/>
+      <c r="AN60" s="42"/>
+      <c r="AO60" s="42"/>
+      <c r="AP60" s="42"/>
+      <c r="AQ60" s="42"/>
+      <c r="AR60" s="42"/>
+      <c r="AS60" s="42"/>
+      <c r="AT60" s="42"/>
+      <c r="AU60" s="42"/>
+      <c r="AV60" s="42"/>
+      <c r="AW60" s="42"/>
+      <c r="AX60" s="42"/>
+      <c r="AY60" s="42"/>
+      <c r="AZ60" s="42"/>
+      <c r="BA60" s="42"/>
+      <c r="BB60" s="42"/>
+      <c r="BC60" s="42"/>
+      <c r="BD60" s="42"/>
+      <c r="BE60" s="42"/>
+      <c r="BF60" s="42"/>
+      <c r="BG60" s="42"/>
+      <c r="BH60" s="42"/>
+      <c r="BI60" s="42"/>
+      <c r="BJ60" s="42"/>
+      <c r="BK60" s="42"/>
+      <c r="BL60" s="42"/>
+      <c r="BM60" s="42"/>
+      <c r="BN60" s="42"/>
+      <c r="BO60" s="42"/>
+      <c r="BP60" s="42"/>
+      <c r="BQ60" s="42"/>
+      <c r="BR60" s="42"/>
+      <c r="BS60" s="42"/>
+      <c r="BT60" s="42"/>
+      <c r="BU60" s="42"/>
+      <c r="BV60" s="42"/>
+      <c r="BW60" s="42"/>
+      <c r="BX60" s="42"/>
+      <c r="BY60" s="42"/>
+      <c r="BZ60" s="42"/>
+      <c r="CA60" s="42"/>
+      <c r="CB60" s="42"/>
+      <c r="CC60" s="42"/>
+      <c r="CD60" s="42"/>
+      <c r="CE60" s="42"/>
+      <c r="CF60" s="42"/>
+      <c r="CG60" s="42"/>
+      <c r="CH60" s="42"/>
+      <c r="CI60" s="42"/>
+      <c r="CJ60" s="42"/>
+      <c r="CK60" s="42"/>
+      <c r="CL60" s="42"/>
+      <c r="CM60" s="42"/>
+      <c r="CN60" s="42"/>
+      <c r="CO60" s="42"/>
+      <c r="CP60" s="42"/>
+      <c r="CQ60" s="42"/>
+      <c r="CR60" s="42"/>
+      <c r="CS60" s="42"/>
+      <c r="CT60" s="42"/>
+      <c r="CU60" s="42"/>
+      <c r="CV60" s="42"/>
+      <c r="CW60" s="42"/>
+      <c r="CX60" s="42"/>
+      <c r="CY60" s="42"/>
+      <c r="CZ60" s="42"/>
+      <c r="DA60" s="42"/>
+      <c r="DB60" s="42"/>
+      <c r="DC60" s="42"/>
+      <c r="DD60" s="42"/>
+      <c r="DE60" s="42"/>
+      <c r="DF60" s="42"/>
+      <c r="DG60" s="42"/>
+      <c r="DH60" s="42"/>
+      <c r="DI60" s="42"/>
+      <c r="DJ60" s="42"/>
+      <c r="DK60" s="42"/>
+      <c r="DL60" s="42"/>
+      <c r="DM60" s="42"/>
+      <c r="DN60" s="42"/>
+      <c r="DO60" s="42"/>
+      <c r="DP60" s="42"/>
+      <c r="DQ60" s="42"/>
+      <c r="DR60" s="42"/>
+      <c r="DS60" s="42"/>
+      <c r="DT60" s="42"/>
+      <c r="DU60" s="42"/>
+      <c r="DV60" s="42"/>
+      <c r="DW60" s="42"/>
+      <c r="DX60" s="42"/>
+      <c r="DY60" s="42"/>
+      <c r="DZ60" s="42"/>
+      <c r="EA60" s="42"/>
+      <c r="EB60" s="42"/>
+      <c r="EC60" s="42"/>
+      <c r="ED60" s="42"/>
+      <c r="EE60" s="42"/>
+      <c r="EF60" s="42"/>
+      <c r="EG60" s="42"/>
+      <c r="EH60" s="42"/>
+      <c r="EI60" s="42"/>
+      <c r="EJ60" s="42"/>
+      <c r="EK60" s="42"/>
+      <c r="EL60" s="42"/>
+      <c r="EM60" s="42"/>
+      <c r="EN60" s="42"/>
+      <c r="EO60" s="42"/>
+      <c r="EP60" s="42"/>
+      <c r="EQ60" s="42"/>
+      <c r="ER60" s="42"/>
+      <c r="ES60" s="42"/>
+      <c r="ET60" s="42"/>
+      <c r="EU60" s="42"/>
+      <c r="EV60" s="42"/>
+      <c r="EW60" s="42"/>
+      <c r="EX60" s="42"/>
+      <c r="EY60" s="42"/>
+      <c r="EZ60" s="42"/>
+      <c r="FA60" s="42"/>
+      <c r="FB60" s="42"/>
+      <c r="FC60" s="42"/>
+      <c r="FD60" s="42"/>
+      <c r="FE60" s="42"/>
+      <c r="FF60" s="42"/>
+      <c r="FG60" s="42"/>
+      <c r="FH60" s="42"/>
+      <c r="FI60" s="42"/>
+      <c r="FJ60" s="42"/>
+      <c r="FK60" s="42"/>
+      <c r="FL60" s="42"/>
+      <c r="FM60" s="42"/>
+      <c r="FN60" s="42"/>
+      <c r="FO60" s="42"/>
+      <c r="FP60" s="42"/>
+      <c r="FQ60" s="42"/>
+      <c r="FR60" s="42"/>
+      <c r="FS60" s="42"/>
+      <c r="FT60" s="42"/>
+      <c r="FU60" s="42"/>
+      <c r="FV60" s="42"/>
+      <c r="FW60" s="42"/>
+      <c r="FX60" s="42"/>
+      <c r="FY60" s="42"/>
+      <c r="FZ60" s="42"/>
+      <c r="GA60" s="42"/>
+      <c r="GB60" s="42"/>
+      <c r="GC60" s="42"/>
+      <c r="GD60" s="42"/>
+      <c r="GE60" s="42"/>
+      <c r="GF60" s="42"/>
+      <c r="GG60" s="42"/>
+      <c r="GH60" s="42"/>
+      <c r="GI60" s="42"/>
+      <c r="GJ60" s="42"/>
+      <c r="GK60" s="42"/>
+      <c r="GL60" s="42"/>
+      <c r="GM60" s="42"/>
+      <c r="GN60" s="42"/>
+      <c r="GO60" s="42"/>
+      <c r="GP60" s="42"/>
+      <c r="GQ60" s="42"/>
+      <c r="GR60" s="42"/>
+      <c r="GS60" s="42"/>
+      <c r="GT60" s="42"/>
+      <c r="GU60" s="42"/>
+      <c r="GV60" s="42"/>
+      <c r="GW60" s="42"/>
+      <c r="GX60" s="42"/>
+      <c r="GY60" s="42"/>
+      <c r="GZ60" s="42"/>
+      <c r="HA60" s="42"/>
+      <c r="HB60" s="42"/>
+      <c r="HC60" s="42"/>
+      <c r="HD60" s="42"/>
+      <c r="HE60" s="42"/>
+      <c r="HF60" s="42"/>
+      <c r="HG60" s="42"/>
+      <c r="HH60" s="42"/>
+      <c r="HI60" s="42"/>
+      <c r="HJ60" s="42"/>
+      <c r="HK60" s="42"/>
+      <c r="HL60" s="42"/>
+      <c r="HM60" s="42"/>
+      <c r="HN60" s="42"/>
+      <c r="HO60" s="42"/>
+      <c r="HP60" s="42"/>
+      <c r="HQ60" s="42"/>
+      <c r="HR60" s="42"/>
+      <c r="HS60" s="42"/>
+      <c r="HT60" s="42"/>
+      <c r="HU60" s="42"/>
+      <c r="HV60" s="42"/>
+      <c r="HW60" s="42"/>
+      <c r="HX60" s="42"/>
+      <c r="HY60" s="42"/>
+      <c r="HZ60" s="42"/>
+      <c r="IA60" s="42"/>
+      <c r="IB60" s="42"/>
+      <c r="IC60" s="42"/>
+      <c r="ID60" s="42"/>
+      <c r="IE60" s="42"/>
+      <c r="IF60" s="42"/>
+      <c r="IG60" s="42"/>
+      <c r="IH60" s="42"/>
+      <c r="II60" s="42"/>
+      <c r="IJ60" s="42"/>
+      <c r="IK60" s="42"/>
+      <c r="IL60" s="42"/>
+      <c r="IM60" s="42"/>
+      <c r="IN60" s="42"/>
+      <c r="IO60" s="42"/>
+      <c r="IP60" s="42"/>
+      <c r="IQ60" s="42"/>
+      <c r="IR60" s="42"/>
+      <c r="IS60" s="42"/>
+      <c r="IT60" s="42"/>
+      <c r="IU60" s="42"/>
+      <c r="IV60" s="42"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -23326,7 +24486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
@@ -26813,10 +27973,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -27699,6 +28859,46 @@
       <c r="S20" s="7"/>
       <c r="T20" s="8"/>
     </row>
+    <row r="21" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B21" s="10"/>
+      <c r="C21" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>507</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>508</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>508</v>
+      </c>
+      <c r="G21" s="6">
+        <v>1</v>
+      </c>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q21" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="R21" s="7"/>
+      <c r="S21" s="7"/>
+      <c r="T21" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180599999999998" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
RDM-2804 updated functional tests
</commit_message>
<xml_diff>
--- a/test/resources/definitionsFiles/fe-automation-definition-v06_collection_view_2804.xlsx
+++ b/test/resources/definitionsFiles/fe-automation-definition-v06_collection_view_2804.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ganganna/moj/code/ccd-case-management-web/test/resources/definitionsFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B459D626-3BDC-1947-85CC-29DDDEB38C48}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7BB4AF-191F-8945-9F1F-52327B41ACE7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="520" windowWidth="28600" windowHeight="17380" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="640" windowWidth="24140" windowHeight="17240" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2239" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2244" uniqueCount="520">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1539,9 +1539,6 @@
     <t>MySchool.ProvidesAutisticChildrenSupport="Yes" AND MySchool.Class.ClassMembers.Children.IsAutistic="Yes"</t>
   </si>
   <si>
-    <t>MySchool.Class.ClassMembers.Children.IsAutistic="Yes"</t>
-  </si>
-  <si>
     <t>Child full name (UPDATED)</t>
   </si>
   <si>
@@ -1641,9 +1638,6 @@
     <t>TextField4="orValue1" OR TextField4="orValue2"</t>
   </si>
   <si>
-    <t>TextField6!="orValue1" OR TextField6!="orValue2"</t>
-  </si>
-  <si>
     <t>createCaseAnd</t>
   </si>
   <si>
@@ -1669,6 +1663,24 @@
   </si>
   <si>
     <t>TextField8="orValue1" AND TextField9="orValue2"</t>
+  </si>
+  <si>
+    <t>Class.ClassMembers.Children.NeedsSupportOR</t>
+  </si>
+  <si>
+    <t>MySchool.Class.ClassName="orTestSchool" OR MySchool.Class.ClassName="orTestSchool1"</t>
+  </si>
+  <si>
+    <t>TextField8="orValue1" AND TextField9="orValue3"</t>
+  </si>
+  <si>
+    <t>TextField4="orValue4" OR TextField4="orValue5"</t>
+  </si>
+  <si>
+    <t>TextField6!="orValue4" OR TextField6="orValue1"</t>
+  </si>
+  <si>
+    <t>TextField6="orValue4" OR TextField6!="orValue1"</t>
   </si>
 </sst>
 </file>
@@ -3631,8 +3643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AD55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B23" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G15" workbookViewId="0">
+      <selection activeCell="M48" sqref="M48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.25" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3798,7 +3810,7 @@
         <v>215</v>
       </c>
       <c r="N3" s="138" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="O3" s="8" t="s">
         <v>216</v>
@@ -4900,10 +4912,10 @@
         <v>285</v>
       </c>
       <c r="D25" s="106" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E25" s="59" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F25" s="120">
         <v>1</v>
@@ -4912,10 +4924,10 @@
         <v>218</v>
       </c>
       <c r="H25" s="106" t="s">
+        <v>486</v>
+      </c>
+      <c r="I25" s="106" t="s">
         <v>487</v>
-      </c>
-      <c r="I25" s="106" t="s">
-        <v>488</v>
       </c>
       <c r="J25" s="121">
         <v>1</v>
@@ -4951,10 +4963,10 @@
         <v>285</v>
       </c>
       <c r="D26" s="96" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E26" s="138" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="F26" s="146">
         <v>1</v>
@@ -4963,10 +4975,10 @@
         <v>218</v>
       </c>
       <c r="H26" s="138" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I26" s="138" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="J26" s="141">
         <v>1</v>
@@ -4975,7 +4987,7 @@
       <c r="L26" s="142"/>
       <c r="M26" s="142"/>
       <c r="N26" s="143" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="O26" s="137" t="s">
         <v>195</v>
@@ -5976,7 +5988,7 @@
         <v>398</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E46" s="8" t="s">
         <v>335</v>
@@ -6027,7 +6039,7 @@
         <v>398</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E47" s="8" t="s">
         <v>336</v>
@@ -6050,7 +6062,7 @@
       <c r="K47" s="7"/>
       <c r="L47" s="7"/>
       <c r="M47" s="7" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="N47" s="142"/>
       <c r="O47" s="8" t="s">
@@ -6080,10 +6092,10 @@
         <v>398</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F48" s="23">
         <v>2</v>
@@ -6102,7 +6114,7 @@
       </c>
       <c r="K48" s="7"/>
       <c r="L48" s="7" t="s">
-        <v>505</v>
+        <v>517</v>
       </c>
       <c r="M48" s="7"/>
       <c r="N48" s="142"/>
@@ -6133,7 +6145,7 @@
         <v>398</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E49" s="8" t="s">
         <v>338</v>
@@ -6184,7 +6196,7 @@
         <v>398</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E50" s="8" t="s">
         <v>339</v>
@@ -6207,7 +6219,7 @@
       <c r="K50" s="7"/>
       <c r="L50" s="7"/>
       <c r="M50" s="22" t="s">
-        <v>506</v>
+        <v>519</v>
       </c>
       <c r="N50" s="142"/>
       <c r="O50" s="8" t="s">
@@ -6237,10 +6249,10 @@
         <v>398</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F51" s="23">
         <v>2</v>
@@ -6259,7 +6271,7 @@
       </c>
       <c r="K51" s="7"/>
       <c r="L51" s="7" t="s">
-        <v>506</v>
+        <v>518</v>
       </c>
       <c r="M51" s="7"/>
       <c r="N51" s="142"/>
@@ -6290,10 +6302,10 @@
         <v>398</v>
       </c>
       <c r="D52" s="8" t="s">
+        <v>505</v>
+      </c>
+      <c r="E52" s="8" t="s">
         <v>507</v>
-      </c>
-      <c r="E52" s="8" t="s">
-        <v>509</v>
       </c>
       <c r="F52" s="23">
         <v>1</v>
@@ -6341,10 +6353,10 @@
         <v>398</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="F53" s="23">
         <v>1</v>
@@ -6392,10 +6404,10 @@
         <v>398</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="F54" s="23">
         <v>2</v>
@@ -6415,7 +6427,7 @@
       <c r="K54" s="7"/>
       <c r="L54" s="7"/>
       <c r="M54" s="7" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="N54" s="142"/>
       <c r="O54" s="8" t="s">
@@ -6445,10 +6457,10 @@
         <v>398</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F55" s="23">
         <v>2</v>
@@ -6467,7 +6479,7 @@
       </c>
       <c r="K55" s="7"/>
       <c r="L55" s="7" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="M55" s="7"/>
       <c r="N55" s="142"/>
@@ -7878,7 +7890,7 @@
         <v>42736</v>
       </c>
       <c r="C5" s="124" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>272</v>
@@ -7903,7 +7915,7 @@
         <v>42736</v>
       </c>
       <c r="C6" s="124" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>272</v>
@@ -8531,7 +8543,7 @@
         <v>397</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E17" t="s">
         <v>271</v>
@@ -8636,7 +8648,7 @@
         <v>275</v>
       </c>
       <c r="D22" s="112" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E22" s="93" t="s">
         <v>271</v>
@@ -8751,7 +8763,7 @@
         <v>285</v>
       </c>
       <c r="D27" s="112" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E27" s="93" t="s">
         <v>271</v>
@@ -8774,7 +8786,7 @@
         <v>285</v>
       </c>
       <c r="D28" s="59" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E28" t="s">
         <v>271</v>
@@ -8797,7 +8809,7 @@
         <v>285</v>
       </c>
       <c r="D29" s="57" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="E29" t="s">
         <v>271</v>
@@ -9050,7 +9062,7 @@
         <v>330</v>
       </c>
       <c r="D40" s="112" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E40" s="93" t="s">
         <v>271</v>
@@ -9165,7 +9177,7 @@
         <v>374</v>
       </c>
       <c r="D45" s="112" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E45" s="93" t="s">
         <v>271</v>
@@ -9211,7 +9223,7 @@
         <v>393</v>
       </c>
       <c r="D47" s="112" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E47" s="93" t="s">
         <v>271</v>
@@ -9565,7 +9577,7 @@
         <v>398</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E52" t="s">
         <v>271</v>
@@ -10089,7 +10101,7 @@
         <v>398</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E54" t="s">
         <v>271</v>
@@ -10351,7 +10363,7 @@
         <v>398</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E55" t="s">
         <v>271</v>
@@ -10397,7 +10409,7 @@
         <v>398</v>
       </c>
       <c r="D57" s="57" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="E57" t="s">
         <v>271</v>
@@ -10420,7 +10432,7 @@
         <v>398</v>
       </c>
       <c r="D58" s="57" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="E58" t="s">
         <v>271</v>
@@ -10443,7 +10455,7 @@
         <v>398</v>
       </c>
       <c r="D59" s="57" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E59" t="s">
         <v>271</v>
@@ -10819,7 +10831,7 @@
         <v>285</v>
       </c>
       <c r="D10" s="96" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E10" s="125" t="s">
         <v>271</v>
@@ -10842,7 +10854,7 @@
         <v>285</v>
       </c>
       <c r="D11" s="96" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E11" s="125" t="s">
         <v>271</v>
@@ -11049,7 +11061,7 @@
         <v>398</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E20" s="54" t="s">
         <v>271</v>
@@ -11072,7 +11084,7 @@
         <v>398</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E21" s="54" t="s">
         <v>271</v>
@@ -11095,7 +11107,7 @@
         <v>398</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="E22" s="54" t="s">
         <v>271</v>
@@ -12590,14 +12602,14 @@
         <v>397</v>
       </c>
       <c r="D17" s="90" t="s">
+        <v>474</v>
+      </c>
+      <c r="E17" s="90" t="s">
         <v>475</v>
-      </c>
-      <c r="E17" s="90" t="s">
-        <v>476</v>
       </c>
       <c r="F17" s="91"/>
       <c r="G17" s="90" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="H17" s="91"/>
       <c r="I17" s="91"/>
@@ -13940,14 +13952,14 @@
         <v>275</v>
       </c>
       <c r="D22" s="90" t="s">
+        <v>474</v>
+      </c>
+      <c r="E22" s="90" t="s">
         <v>475</v>
-      </c>
-      <c r="E22" s="90" t="s">
-        <v>476</v>
       </c>
       <c r="F22" s="91"/>
       <c r="G22" s="90" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="H22" s="91"/>
       <c r="I22" s="91"/>
@@ -15022,14 +15034,14 @@
         <v>285</v>
       </c>
       <c r="D26" s="90" t="s">
+        <v>474</v>
+      </c>
+      <c r="E26" s="90" t="s">
         <v>475</v>
-      </c>
-      <c r="E26" s="90" t="s">
-        <v>476</v>
       </c>
       <c r="F26" s="91"/>
       <c r="G26" s="90" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="H26" s="91"/>
       <c r="I26" s="91"/>
@@ -15562,10 +15574,10 @@
         <v>285</v>
       </c>
       <c r="D28" s="59" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E28" s="57" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="57" t="s">
@@ -15834,10 +15846,10 @@
         <v>285</v>
       </c>
       <c r="D29" s="138" t="s">
+        <v>478</v>
+      </c>
+      <c r="E29" s="138" t="s">
         <v>479</v>
-      </c>
-      <c r="E29" s="138" t="s">
-        <v>480</v>
       </c>
       <c r="F29" s="142"/>
       <c r="G29" s="137" t="s">
@@ -18810,14 +18822,14 @@
         <v>330</v>
       </c>
       <c r="D40" s="90" t="s">
+        <v>474</v>
+      </c>
+      <c r="E40" s="90" t="s">
         <v>475</v>
-      </c>
-      <c r="E40" s="90" t="s">
-        <v>476</v>
       </c>
       <c r="F40" s="91"/>
       <c r="G40" s="90" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="H40" s="91"/>
       <c r="I40" s="91"/>
@@ -20160,14 +20172,14 @@
         <v>374</v>
       </c>
       <c r="D45" s="90" t="s">
+        <v>474</v>
+      </c>
+      <c r="E45" s="90" t="s">
         <v>475</v>
-      </c>
-      <c r="E45" s="90" t="s">
-        <v>476</v>
       </c>
       <c r="F45" s="91"/>
       <c r="G45" s="90" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="H45" s="91"/>
       <c r="I45" s="91"/>
@@ -20702,14 +20714,14 @@
         <v>393</v>
       </c>
       <c r="D47" s="90" t="s">
+        <v>474</v>
+      </c>
+      <c r="E47" s="90" t="s">
         <v>475</v>
-      </c>
-      <c r="E47" s="90" t="s">
-        <v>476</v>
       </c>
       <c r="F47" s="91"/>
       <c r="G47" s="90" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="H47" s="91"/>
       <c r="I47" s="91"/>
@@ -22322,10 +22334,10 @@
         <v>398</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F53" s="7"/>
       <c r="G53" s="8" t="s">
@@ -23132,10 +23144,10 @@
         <v>398</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F56" s="7"/>
       <c r="G56" s="8" t="s">
@@ -23402,14 +23414,14 @@
         <v>398</v>
       </c>
       <c r="D57" s="90" t="s">
+        <v>474</v>
+      </c>
+      <c r="E57" s="90" t="s">
         <v>475</v>
-      </c>
-      <c r="E57" s="90" t="s">
-        <v>476</v>
       </c>
       <c r="F57" s="91"/>
       <c r="G57" s="90" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="H57" s="91"/>
       <c r="I57" s="91"/>
@@ -23672,10 +23684,10 @@
         <v>398</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="F58" s="7"/>
       <c r="G58" s="8" t="s">
@@ -23942,10 +23954,10 @@
         <v>398</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="F59" s="7"/>
       <c r="G59" s="8" t="s">
@@ -24212,10 +24224,10 @@
         <v>398</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="F60" s="7"/>
       <c r="G60" s="8" t="s">
@@ -24486,7 +24498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
@@ -25672,10 +25684,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E561A8A-480D-6D45-8F14-5D4A9428A511}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -25686,11 +25698,11 @@
     <col min="4" max="4" width="23.5" customWidth="1"/>
     <col min="5" max="5" width="18.6640625" customWidth="1"/>
     <col min="6" max="6" width="57.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.83203125" customWidth="1"/>
     <col min="8" max="8" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="89.6640625" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" customWidth="1"/>
+    <col min="11" max="11" width="97.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.2">
@@ -25900,10 +25912,10 @@
         <v>466</v>
       </c>
       <c r="G8" s="84" t="s">
+        <v>472</v>
+      </c>
+      <c r="H8" s="84" t="s">
         <v>473</v>
-      </c>
-      <c r="H8" s="84" t="s">
-        <v>474</v>
       </c>
       <c r="I8">
         <v>4</v>
@@ -26006,8 +26018,31 @@
       <c r="J12" s="84" t="s">
         <v>438</v>
       </c>
-      <c r="K12" s="84" t="s">
-        <v>472</v>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A13" s="85">
+        <v>43101</v>
+      </c>
+      <c r="C13" t="s">
+        <v>436</v>
+      </c>
+      <c r="D13" s="84" t="s">
+        <v>453</v>
+      </c>
+      <c r="E13" s="84" t="s">
+        <v>455</v>
+      </c>
+      <c r="F13" s="84" t="s">
+        <v>514</v>
+      </c>
+      <c r="I13">
+        <v>10</v>
+      </c>
+      <c r="J13" s="84" t="s">
+        <v>438</v>
+      </c>
+      <c r="K13" s="84" t="s">
+        <v>515</v>
       </c>
     </row>
   </sheetData>
@@ -26469,7 +26504,7 @@
         <v>154</v>
       </c>
       <c r="L3" s="147" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
@@ -26518,16 +26553,16 @@
         <v>157</v>
       </c>
       <c r="E5" s="113" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F5" s="114" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G5" s="135">
         <v>1</v>
       </c>
       <c r="H5" s="112" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="I5" s="115">
         <v>1</v>
@@ -26614,16 +26649,16 @@
         <v>157</v>
       </c>
       <c r="E8" s="113" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F8" s="114" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G8" s="135">
         <v>1</v>
       </c>
       <c r="H8" s="112" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="I8" s="115">
         <v>1</v>
@@ -26646,16 +26681,16 @@
         <v>157</v>
       </c>
       <c r="E9" s="128" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F9" s="130" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G9" s="135">
         <v>1</v>
       </c>
       <c r="H9" s="129" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="I9" s="131">
         <v>1</v>
@@ -27068,16 +27103,16 @@
         <v>157</v>
       </c>
       <c r="E22" s="113" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F22" s="114" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G22" s="135">
         <v>1</v>
       </c>
       <c r="H22" s="112" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="I22" s="115">
         <v>1</v>
@@ -27100,16 +27135,16 @@
         <v>157</v>
       </c>
       <c r="E23" s="113" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F23" s="114" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G23" s="135">
         <v>1</v>
       </c>
       <c r="H23" s="59" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I23" s="115">
         <v>1</v>
@@ -27117,7 +27152,7 @@
       <c r="J23" s="116"/>
       <c r="K23" s="116"/>
       <c r="L23" s="143" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="M23" s="116"/>
       <c r="N23" s="116"/>
@@ -27134,16 +27169,16 @@
         <v>157</v>
       </c>
       <c r="E24" s="138" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F24" s="139" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="G24" s="140">
         <v>2</v>
       </c>
       <c r="H24" s="138" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="I24" s="141">
         <v>2</v>
@@ -27151,7 +27186,7 @@
       <c r="J24" s="142"/>
       <c r="K24" s="142"/>
       <c r="L24" s="143" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="M24" s="142"/>
       <c r="N24" s="142"/>
@@ -27296,16 +27331,16 @@
         <v>157</v>
       </c>
       <c r="E29" s="130" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F29" s="130" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G29" s="131">
         <v>1</v>
       </c>
       <c r="H29" s="128" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="I29" s="131">
         <v>4</v>
@@ -27360,16 +27395,16 @@
         <v>157</v>
       </c>
       <c r="E31" s="114" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F31" s="114" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G31" s="135">
         <v>1</v>
       </c>
       <c r="H31" s="113" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="I31" s="115">
         <v>1</v>
@@ -27501,7 +27536,7 @@
         <v>2</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="I35" s="6">
         <v>1</v>
@@ -27565,7 +27600,7 @@
         <v>2</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="I37" s="6">
         <v>1</v>
@@ -27588,16 +27623,16 @@
         <v>157</v>
       </c>
       <c r="E38" s="103" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F38" s="103" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G38" s="135">
         <v>1</v>
       </c>
       <c r="H38" s="103" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="I38" s="117">
         <v>1</v>
@@ -28370,13 +28405,13 @@
         <v>285</v>
       </c>
       <c r="D9" s="96" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E9" s="109" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F9" s="109" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="G9" s="122">
         <v>2</v>
@@ -28410,13 +28445,13 @@
         <v>285</v>
       </c>
       <c r="D10" s="96" t="s">
+        <v>492</v>
+      </c>
+      <c r="E10" s="109" t="s">
         <v>493</v>
       </c>
-      <c r="E10" s="109" t="s">
-        <v>494</v>
-      </c>
       <c r="F10" s="109" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="G10" s="122">
         <v>3</v>
@@ -28788,13 +28823,13 @@
         <v>398</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G19" s="6">
         <v>1</v>
@@ -28828,13 +28863,13 @@
         <v>398</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G20" s="6">
         <v>1</v>
@@ -28868,13 +28903,13 @@
         <v>398</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="G21" s="6">
         <v>1</v>

</xml_diff>